<commit_message>
Added ignoring headers. Started writing data to a file. Sleep
</commit_message>
<xml_diff>
--- a/bin/Debug/Test.xlsx
+++ b/bin/Debug/Test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lifec\Desktop\DataTable(Intima)\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0CE87E-168C-497E-8BC2-D71682580689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBACBE69-35AB-4EB3-A5B1-1CD0CFAF0C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,49 +27,49 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
-    <t>DataTime</t>
-  </si>
-  <si>
-    <t>TagName</t>
+    <t>Boiler.P1.Value</t>
+  </si>
+  <si>
+    <t>Boiler.P2.Value</t>
+  </si>
+  <si>
+    <t>Boiler.T1.Value</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Boiler.P3.Value</t>
+  </si>
+  <si>
+    <t>Boiler.P4.Value</t>
+  </si>
+  <si>
+    <t>Boiler.P5.Value</t>
+  </si>
+  <si>
+    <t>Boiler.T2.Value</t>
+  </si>
+  <si>
+    <t>Boiler.T4.Value</t>
+  </si>
+  <si>
+    <t>Boiler.T3.Value</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Date time</t>
+  </si>
+  <si>
+    <t>Tag type</t>
   </si>
   <si>
     <t>Type</t>
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>Boiler.P1.Value</t>
-  </si>
-  <si>
-    <t>Boiler.P2.Value</t>
-  </si>
-  <si>
-    <t>Boiler.T1.Value</t>
-  </si>
-  <si>
-    <t>Float</t>
-  </si>
-  <si>
-    <t>Boiler.P3.Value</t>
-  </si>
-  <si>
-    <t>Boiler.P4.Value</t>
-  </si>
-  <si>
-    <t>Boiler.P5.Value</t>
-  </si>
-  <si>
-    <t>Boiler.T2.Value</t>
-  </si>
-  <si>
-    <t>Boiler.T4.Value</t>
-  </si>
-  <si>
-    <t>Boiler.T3.Value</t>
-  </si>
-  <si>
-    <t>Integer</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -125,6 +125,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -405,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,147 +417,197 @@
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>44185.375</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44185.375</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3">
         <v>3.4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>44185.375694444447</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>44185.375925925924</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>44185.37604166667</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+      <c r="B5" t="s">
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>44185.376388888886</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>44185.376562500001</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
+      <c r="B7" t="s">
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>44185.376736111109</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
+      <c r="B8" t="s">
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="5">
         <v>1.002</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
         <v>44185.376851851855</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D9" s="6">
         <v>12.000500000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>44185.377025462964</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
+      <c r="B10" t="s">
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4">
         <v>9</v>
       </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J18" s="1"/>
+      <c r="K18" s="2"/>
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+      <c r="K19" s="2"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+      <c r="K20" s="2"/>
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J21" s="1"/>
+      <c r="K21" s="2"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+      <c r="K22" s="2"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J23" s="1"/>
+      <c r="K23" s="2"/>
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J24" s="1"/>
+      <c r="K24" s="2"/>
+      <c r="M24" s="6"/>
+    </row>
+    <row r="25" spans="10:13" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+      <c r="K25" s="2"/>
+      <c r="M25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>